<commit_message>
docs bijna klaar voor review
</commit_message>
<xml_diff>
--- a/IMKL2.x/1. dataspecificatie/IMKL_Modeldoc-changelog.xlsx
+++ b/IMKL2.x/1. dataspecificatie/IMKL_Modeldoc-changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjanssen\Documents\GitHub\imkl2015-review\IMKL2.x\1. dataspecificatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97CAE91-5D3D-42CF-B990-B906B948CD67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B94EDE-CCCB-41BC-BAD7-87B412F130F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{894B1FF5-8DFC-4651-A7C4-67B2EE5B0E46}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Changelog" sheetId="1" r:id="rId1"/>
     <sheet name="Blad1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -654,7 +654,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -711,7 +711,9 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="6">
+        <v>43976</v>
+      </c>
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
@@ -722,7 +724,9 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="6">
+        <v>43976</v>
+      </c>
       <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
@@ -733,7 +737,9 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
+      <c r="A6" s="6">
+        <v>43976</v>
+      </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
         <v>19</v>
@@ -742,7 +748,9 @@
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:9" ht="24" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
+      <c r="A7" s="6">
+        <v>43976</v>
+      </c>
       <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
@@ -753,7 +761,9 @@
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6">
+        <v>43976</v>
+      </c>
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
@@ -764,7 +774,9 @@
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:9" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A9" s="6"/>
+      <c r="A9" s="6">
+        <v>43976</v>
+      </c>
       <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
@@ -777,7 +789,9 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:9" ht="115.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
+      <c r="A10" s="6">
+        <v>43976</v>
+      </c>
       <c r="B10" s="6" t="s">
         <v>24</v>
       </c>
@@ -2136,21 +2150,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003ADD3040E3157B4E913BCA65F34844D7" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c1765059aa1475931adc12138fdcfd8c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="aafb19fa-82be-411d-a6df-c75e9235a4ea" xmlns:ns3="3dfebdfe-2b22-40ba-8672-9fbc9b4066c4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="42d79c55539af1f9f274032ce6041302" ns2:_="" ns3:_="">
     <xsd:import namespace="aafb19fa-82be-411d-a6df-c75e9235a4ea"/>
@@ -2353,24 +2352,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1489CD-B12A-4704-A7E2-006D773FFFBF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0C9FDDB-2830-4DD6-A847-D844746B12F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2387,4 +2384,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7893A73B-81F0-482A-B793-D93E5F8DCA71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB1489CD-B12A-4704-A7E2-006D773FFFBF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>